<commit_message>
Objeto y signatura arreglada
</commit_message>
<xml_diff>
--- a/Docs/Documentación de tablas SQL.xlsx
+++ b/Docs/Documentación de tablas SQL.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\Universidad\Cuarto Semestre\Iter3Sistrans\Iteracion2-Sistrans\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Code\University\Iteración3\Iteracion2-Sistrans\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="225">
   <si>
     <t>Nombre</t>
   </si>
@@ -623,9 +623,6 @@
     <t>Valor binario (booleano) que representa si ya se entregó (1) o no la orden (0)</t>
   </si>
   <si>
-    <t>Es 1 o 0</t>
-  </si>
-  <si>
     <t>TIempoR</t>
   </si>
   <si>
@@ -681,13 +678,31 @@
   </si>
   <si>
     <t>Restaurante_nombre, producto_nombre</t>
+  </si>
+  <si>
+    <t>Menu_Checkout</t>
+  </si>
+  <si>
+    <t>Tabla que modela la relación muchos a muchos entre los registros órdenes de compras y los menús en RotondAndes.</t>
+  </si>
+  <si>
+    <t>mayor a cero, NN</t>
+  </si>
+  <si>
+    <t>Nombre del restaurante al que pertenece el producto de la compra</t>
+  </si>
+  <si>
+    <t>Es 1 o 0, NN</t>
+  </si>
+  <si>
+    <t>longitud mayor a 5, NN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,6 +720,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1112,7 +1135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1268,6 +1291,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1277,12 +1309,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1382,6 +1418,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1417,6 +1470,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1593,10 +1663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F182"/>
+  <dimension ref="A1:F192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:D42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,37 +1677,37 @@
     <col min="4" max="4" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="61"/>
-    </row>
-    <row r="2" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="57"/>
+      <c r="D1" s="58"/>
+    </row>
+    <row r="2" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="57"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="59"/>
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="59"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="61"/>
+      <c r="D3" s="62"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -1651,7 +1721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>0</v>
       </c>
@@ -1665,7 +1735,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>1</v>
       </c>
@@ -1676,10 +1746,11 @@
         <v>62</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+      <c r="F6" s="66"/>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>56</v>
       </c>
@@ -1690,10 +1761,10 @@
         <v>64</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>57</v>
       </c>
@@ -1707,38 +1778,38 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="57"/>
+      <c r="D11" s="58"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="57"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="59"/>
+      <c r="D12" s="60"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="58"/>
-      <c r="D13" s="59"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="61"/>
+      <c r="D13" s="62"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>3</v>
       </c>
@@ -1752,7 +1823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>69</v>
       </c>
@@ -1771,31 +1842,31 @@
       <c r="A18" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="60"/>
-      <c r="D18" s="61"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="58"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="56"/>
-      <c r="D19" s="57"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="60"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="58"/>
-      <c r="D20" s="59"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="62"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
@@ -1911,31 +1982,31 @@
       <c r="A30" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="60"/>
-      <c r="D30" s="61"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="58"/>
     </row>
     <row r="31" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="C31" s="56"/>
-      <c r="D31" s="57"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="60"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="59"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="62"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
@@ -2012,31 +2083,31 @@
       <c r="A40" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="60" t="s">
+      <c r="B40" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="60"/>
-      <c r="D40" s="61"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="58"/>
     </row>
     <row r="41" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="56" t="s">
+      <c r="B41" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="56"/>
-      <c r="D41" s="57"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="60"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="58" t="s">
-        <v>219</v>
-      </c>
-      <c r="C42" s="58"/>
-      <c r="D42" s="59"/>
+      <c r="B42" s="61" t="s">
+        <v>218</v>
+      </c>
+      <c r="C42" s="61"/>
+      <c r="D42" s="62"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
@@ -2074,7 +2145,7 @@
         <v>95</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>97</v>
@@ -2082,13 +2153,13 @@
     </row>
     <row r="46" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B46" s="13" t="s">
         <v>153</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>83</v>
@@ -2099,31 +2170,31 @@
       <c r="A49" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="60" t="s">
+      <c r="B49" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C49" s="60"/>
-      <c r="D49" s="61"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="58"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B50" s="56" t="s">
+      <c r="B50" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="56"/>
-      <c r="D50" s="57"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="60"/>
     </row>
     <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="58" t="s">
+      <c r="B51" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C51" s="58"/>
-      <c r="D51" s="59"/>
+      <c r="C51" s="61"/>
+      <c r="D51" s="62"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
@@ -2200,31 +2271,31 @@
       <c r="A59" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B59" s="60" t="s">
+      <c r="B59" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C59" s="60"/>
-      <c r="D59" s="61"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="58"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="56" t="s">
+      <c r="B60" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="56"/>
-      <c r="D60" s="57"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="60"/>
     </row>
     <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="58" t="s">
+      <c r="B61" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="C61" s="58"/>
-      <c r="D61" s="59"/>
+      <c r="C61" s="61"/>
+      <c r="D61" s="62"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
@@ -2273,31 +2344,31 @@
       <c r="A67" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B67" s="60" t="s">
+      <c r="B67" s="57" t="s">
         <v>117</v>
       </c>
-      <c r="C67" s="60"/>
-      <c r="D67" s="61"/>
+      <c r="C67" s="57"/>
+      <c r="D67" s="58"/>
     </row>
     <row r="68" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B68" s="56" t="s">
+      <c r="B68" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="C68" s="56"/>
-      <c r="D68" s="57"/>
+      <c r="C68" s="59"/>
+      <c r="D68" s="60"/>
     </row>
     <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B69" s="58" t="s">
+      <c r="B69" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="C69" s="58"/>
-      <c r="D69" s="59"/>
+      <c r="C69" s="61"/>
+      <c r="D69" s="62"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
@@ -2335,7 +2406,7 @@
         <v>107</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D72" s="12" t="s">
         <v>97</v>
@@ -2343,13 +2414,13 @@
     </row>
     <row r="73" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>153</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D73" s="14" t="s">
         <v>83</v>
@@ -2360,31 +2431,31 @@
       <c r="A76" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B76" s="60" t="s">
+      <c r="B76" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C76" s="60"/>
-      <c r="D76" s="61"/>
+      <c r="C76" s="57"/>
+      <c r="D76" s="58"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B77" s="56" t="s">
+      <c r="B77" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="C77" s="56"/>
-      <c r="D77" s="57"/>
+      <c r="C77" s="59"/>
+      <c r="D77" s="60"/>
     </row>
     <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B78" s="58" t="s">
+      <c r="B78" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C78" s="58"/>
-      <c r="D78" s="59"/>
+      <c r="C78" s="61"/>
+      <c r="D78" s="62"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
@@ -2503,31 +2574,31 @@
       <c r="A89" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B89" s="60" t="s">
+      <c r="B89" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="C89" s="60"/>
-      <c r="D89" s="61"/>
+      <c r="C89" s="57"/>
+      <c r="D89" s="58"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B90" s="56" t="s">
+      <c r="B90" s="59" t="s">
         <v>149</v>
       </c>
-      <c r="C90" s="56"/>
-      <c r="D90" s="57"/>
+      <c r="C90" s="59"/>
+      <c r="D90" s="60"/>
     </row>
     <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B91" s="58" t="s">
+      <c r="B91" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="C91" s="58"/>
-      <c r="D91" s="59"/>
+      <c r="C91" s="61"/>
+      <c r="D91" s="62"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
@@ -2604,31 +2675,31 @@
       <c r="A99" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B99" s="60" t="s">
+      <c r="B99" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="C99" s="60"/>
-      <c r="D99" s="61"/>
+      <c r="C99" s="57"/>
+      <c r="D99" s="58"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B100" s="56" t="s">
+      <c r="B100" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="C100" s="56"/>
-      <c r="D100" s="57"/>
+      <c r="C100" s="59"/>
+      <c r="D100" s="60"/>
     </row>
     <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B101" s="58" t="s">
+      <c r="B101" s="61" t="s">
         <v>146</v>
       </c>
-      <c r="C101" s="58"/>
-      <c r="D101" s="59"/>
+      <c r="C101" s="61"/>
+      <c r="D101" s="62"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
@@ -2663,31 +2734,31 @@
       <c r="A106" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B106" s="60" t="s">
+      <c r="B106" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="C106" s="60"/>
-      <c r="D106" s="61"/>
+      <c r="C106" s="57"/>
+      <c r="D106" s="58"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B107" s="56" t="s">
+      <c r="B107" s="59" t="s">
         <v>150</v>
       </c>
-      <c r="C107" s="56"/>
-      <c r="D107" s="57"/>
+      <c r="C107" s="59"/>
+      <c r="D107" s="60"/>
     </row>
     <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B108" s="58" t="s">
+      <c r="B108" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C108" s="58"/>
-      <c r="D108" s="59"/>
+      <c r="C108" s="61"/>
+      <c r="D108" s="62"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
@@ -2750,31 +2821,31 @@
       <c r="A115" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B115" s="60" t="s">
+      <c r="B115" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="C115" s="60"/>
-      <c r="D115" s="61"/>
+      <c r="C115" s="57"/>
+      <c r="D115" s="58"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B116" s="56" t="s">
+      <c r="B116" s="59" t="s">
         <v>149</v>
       </c>
-      <c r="C116" s="56"/>
-      <c r="D116" s="57"/>
+      <c r="C116" s="59"/>
+      <c r="D116" s="60"/>
     </row>
     <row r="117" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B117" s="58" t="s">
+      <c r="B117" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="C117" s="58"/>
-      <c r="D117" s="59"/>
+      <c r="C117" s="61"/>
+      <c r="D117" s="62"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
@@ -2851,31 +2922,31 @@
       <c r="A125" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B125" s="60" t="s">
+      <c r="B125" s="57" t="s">
         <v>169</v>
       </c>
-      <c r="C125" s="60"/>
-      <c r="D125" s="61"/>
+      <c r="C125" s="57"/>
+      <c r="D125" s="58"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B126" s="56" t="s">
+      <c r="B126" s="59" t="s">
         <v>170</v>
       </c>
-      <c r="C126" s="56"/>
-      <c r="D126" s="57"/>
+      <c r="C126" s="59"/>
+      <c r="D126" s="60"/>
     </row>
     <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B127" s="58" t="s">
+      <c r="B127" s="61" t="s">
         <v>172</v>
       </c>
-      <c r="C127" s="58"/>
-      <c r="D127" s="59"/>
+      <c r="C127" s="61"/>
+      <c r="D127" s="62"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
@@ -2924,31 +2995,31 @@
       <c r="A133" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B133" s="60" t="s">
+      <c r="B133" s="57" t="s">
         <v>173</v>
       </c>
-      <c r="C133" s="60"/>
-      <c r="D133" s="61"/>
+      <c r="C133" s="57"/>
+      <c r="D133" s="58"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B134" s="56" t="s">
+      <c r="B134" s="59" t="s">
         <v>174</v>
       </c>
-      <c r="C134" s="56"/>
-      <c r="D134" s="57"/>
+      <c r="C134" s="59"/>
+      <c r="D134" s="60"/>
     </row>
     <row r="135" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B135" s="58" t="s">
+      <c r="B135" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="C135" s="58"/>
-      <c r="D135" s="59"/>
+      <c r="C135" s="61"/>
+      <c r="D135" s="62"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
@@ -2997,31 +3068,31 @@
       <c r="A141" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B141" s="60" t="s">
+      <c r="B141" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="C141" s="60"/>
-      <c r="D141" s="61"/>
+      <c r="C141" s="57"/>
+      <c r="D141" s="58"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B142" s="56" t="s">
+      <c r="B142" s="59" t="s">
         <v>178</v>
       </c>
-      <c r="C142" s="56"/>
-      <c r="D142" s="57"/>
+      <c r="C142" s="59"/>
+      <c r="D142" s="60"/>
     </row>
     <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B143" s="58" t="s">
+      <c r="B143" s="61" t="s">
         <v>179</v>
       </c>
-      <c r="C143" s="58"/>
-      <c r="D143" s="59"/>
+      <c r="C143" s="61"/>
+      <c r="D143" s="62"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="8" t="s">
@@ -3070,31 +3141,31 @@
       <c r="A149" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B149" s="60" t="s">
+      <c r="B149" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="C149" s="60"/>
-      <c r="D149" s="61"/>
+      <c r="C149" s="57"/>
+      <c r="D149" s="58"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B150" s="56" t="s">
+      <c r="B150" s="59" t="s">
         <v>182</v>
       </c>
-      <c r="C150" s="56"/>
-      <c r="D150" s="57"/>
+      <c r="C150" s="59"/>
+      <c r="D150" s="60"/>
     </row>
     <row r="151" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B151" s="58" t="s">
+      <c r="B151" s="61" t="s">
         <v>183</v>
       </c>
-      <c r="C151" s="58"/>
-      <c r="D151" s="59"/>
+      <c r="C151" s="61"/>
+      <c r="D151" s="62"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
@@ -3143,31 +3214,31 @@
       <c r="A157" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B157" s="60" t="s">
+      <c r="B157" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="C157" s="60"/>
-      <c r="D157" s="61"/>
+      <c r="C157" s="57"/>
+      <c r="D157" s="58"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B158" s="56" t="s">
+      <c r="B158" s="59" t="s">
         <v>149</v>
       </c>
-      <c r="C158" s="56"/>
-      <c r="D158" s="57"/>
+      <c r="C158" s="59"/>
+      <c r="D158" s="60"/>
     </row>
     <row r="159" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B159" s="58" t="s">
+      <c r="B159" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C159" s="58"/>
-      <c r="D159" s="59"/>
+      <c r="C159" s="61"/>
+      <c r="D159" s="62"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="8" t="s">
@@ -3230,31 +3301,31 @@
       <c r="A166" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B166" s="60" t="s">
+      <c r="B166" s="57" t="s">
         <v>193</v>
       </c>
-      <c r="C166" s="60"/>
-      <c r="D166" s="61"/>
+      <c r="C166" s="57"/>
+      <c r="D166" s="58"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B167" s="56" t="s">
+      <c r="B167" s="59" t="s">
         <v>194</v>
       </c>
-      <c r="C167" s="56"/>
-      <c r="D167" s="57"/>
+      <c r="C167" s="59"/>
+      <c r="D167" s="60"/>
     </row>
     <row r="168" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B168" s="58" t="s">
+      <c r="B168" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="C168" s="58"/>
-      <c r="D168" s="59"/>
+      <c r="C168" s="61"/>
+      <c r="D168" s="62"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="8" t="s">
@@ -3295,18 +3366,18 @@
         <v>199</v>
       </c>
       <c r="D171" s="12" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B172" s="11" t="s">
         <v>63</v>
       </c>
       <c r="C172" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D172" s="12"/>
     </row>
@@ -3318,7 +3389,7 @@
         <v>107</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D173" s="14" t="s">
         <v>168</v>
@@ -3329,31 +3400,31 @@
       <c r="A176" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B176" s="60" t="s">
+      <c r="B176" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="C176" s="57"/>
+      <c r="D176" s="58"/>
+    </row>
+    <row r="177" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B177" s="59" t="s">
         <v>204</v>
       </c>
-      <c r="C176" s="60"/>
-      <c r="D176" s="61"/>
-    </row>
-    <row r="177" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B177" s="56" t="s">
-        <v>205</v>
-      </c>
-      <c r="C177" s="56"/>
-      <c r="D177" s="57"/>
+      <c r="C177" s="59"/>
+      <c r="D177" s="60"/>
     </row>
     <row r="178" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B178" s="58" t="s">
-        <v>207</v>
-      </c>
-      <c r="C178" s="58"/>
-      <c r="D178" s="59"/>
+      <c r="B178" s="61" t="s">
+        <v>206</v>
+      </c>
+      <c r="C178" s="61"/>
+      <c r="D178" s="62"/>
     </row>
     <row r="179" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="50" t="s">
@@ -3371,7 +3442,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="53" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B180" s="54" t="s">
         <v>195</v>
@@ -3380,7 +3451,7 @@
         <v>196</v>
       </c>
       <c r="D180" s="55" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3388,91 +3459,195 @@
         <v>94</v>
       </c>
       <c r="B181" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C181" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="C181" s="11" t="s">
+      <c r="D181" s="12" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A182" s="63" t="s">
+        <v>101</v>
+      </c>
+      <c r="B182" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="C182" s="56" t="s">
+        <v>222</v>
+      </c>
+      <c r="D182" s="65" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="D181" s="12" t="s">
+      <c r="B183" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="C183" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="D183" s="14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B186" s="57" t="s">
+        <v>219</v>
+      </c>
+      <c r="C186" s="57"/>
+      <c r="D186" s="58"/>
+    </row>
+    <row r="187" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B187" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="C187" s="59"/>
+      <c r="D187" s="60"/>
+    </row>
+    <row r="188" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B188" s="61" t="s">
+        <v>206</v>
+      </c>
+      <c r="C188" s="61"/>
+      <c r="D188" s="62"/>
+    </row>
+    <row r="189" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B189" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C189" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D189" s="52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="B190" s="54" t="s">
+        <v>195</v>
+      </c>
+      <c r="C190" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="D190" s="55" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A191" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B191" s="11" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A182" s="21" t="s">
+      <c r="C191" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D191" s="12" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="B192" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="B182" s="13" t="s">
+      <c r="C192" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="C182" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="D182" s="14" t="s">
-        <v>83</v>
+      <c r="D192" s="14" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="63">
+    <mergeCell ref="B186:D186"/>
+    <mergeCell ref="B187:D187"/>
+    <mergeCell ref="B188:D188"/>
+    <mergeCell ref="B167:D167"/>
+    <mergeCell ref="B168:D168"/>
+    <mergeCell ref="B176:D176"/>
+    <mergeCell ref="B177:D177"/>
+    <mergeCell ref="B178:D178"/>
+    <mergeCell ref="B151:D151"/>
+    <mergeCell ref="B157:D157"/>
+    <mergeCell ref="B158:D158"/>
+    <mergeCell ref="B159:D159"/>
+    <mergeCell ref="B166:D166"/>
+    <mergeCell ref="B141:D141"/>
+    <mergeCell ref="B142:D142"/>
+    <mergeCell ref="B143:D143"/>
+    <mergeCell ref="B149:D149"/>
+    <mergeCell ref="B150:D150"/>
+    <mergeCell ref="B126:D126"/>
+    <mergeCell ref="B127:D127"/>
+    <mergeCell ref="B133:D133"/>
+    <mergeCell ref="B134:D134"/>
+    <mergeCell ref="B135:D135"/>
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="B115:D115"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="B125:D125"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="B100:D100"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B106:D106"/>
+    <mergeCell ref="B107:D107"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B30:D30"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B77:D77"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="B91:D91"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="B100:D100"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B106:D106"/>
-    <mergeCell ref="B107:D107"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="B115:D115"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="B125:D125"/>
-    <mergeCell ref="B126:D126"/>
-    <mergeCell ref="B127:D127"/>
-    <mergeCell ref="B133:D133"/>
-    <mergeCell ref="B134:D134"/>
-    <mergeCell ref="B135:D135"/>
-    <mergeCell ref="B141:D141"/>
-    <mergeCell ref="B142:D142"/>
-    <mergeCell ref="B143:D143"/>
-    <mergeCell ref="B149:D149"/>
-    <mergeCell ref="B150:D150"/>
-    <mergeCell ref="B151:D151"/>
-    <mergeCell ref="B157:D157"/>
-    <mergeCell ref="B158:D158"/>
-    <mergeCell ref="B159:D159"/>
-    <mergeCell ref="B166:D166"/>
-    <mergeCell ref="B167:D167"/>
-    <mergeCell ref="B168:D168"/>
-    <mergeCell ref="B176:D176"/>
-    <mergeCell ref="B177:D177"/>
-    <mergeCell ref="B178:D178"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Objeto y signatura arreglada"
This reverts commit baac7dbd1e3d5839fc27c430a54f92f3f90c1972.
</commit_message>
<xml_diff>
--- a/Docs/Documentación de tablas SQL.xlsx
+++ b/Docs/Documentación de tablas SQL.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Code\University\Iteración3\Iteracion2-Sistrans\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\Universidad\Cuarto Semestre\Iter3Sistrans\Iteracion2-Sistrans\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="220">
   <si>
     <t>Nombre</t>
   </si>
@@ -623,6 +623,9 @@
     <t>Valor binario (booleano) que representa si ya se entregó (1) o no la orden (0)</t>
   </si>
   <si>
+    <t>Es 1 o 0</t>
+  </si>
+  <si>
     <t>TIempoR</t>
   </si>
   <si>
@@ -678,31 +681,13 @@
   </si>
   <si>
     <t>Restaurante_nombre, producto_nombre</t>
-  </si>
-  <si>
-    <t>Menu_Checkout</t>
-  </si>
-  <si>
-    <t>Tabla que modela la relación muchos a muchos entre los registros órdenes de compras y los menús en RotondAndes.</t>
-  </si>
-  <si>
-    <t>mayor a cero, NN</t>
-  </si>
-  <si>
-    <t>Nombre del restaurante al que pertenece el producto de la compra</t>
-  </si>
-  <si>
-    <t>Es 1 o 0, NN</t>
-  </si>
-  <si>
-    <t>longitud mayor a 5, NN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -720,14 +705,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1135,7 +1112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1291,34 +1268,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1418,23 +1382,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1470,23 +1417,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1663,10 +1593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F192"/>
+  <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,37 +1607,37 @@
     <col min="4" max="4" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="58"/>
-    </row>
-    <row r="2" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="60"/>
+      <c r="D1" s="61"/>
+    </row>
+    <row r="2" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="60"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="56"/>
+      <c r="D2" s="57"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="62"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="58"/>
+      <c r="D3" s="59"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -1721,7 +1651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>0</v>
       </c>
@@ -1735,7 +1665,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>1</v>
       </c>
@@ -1746,11 +1676,10 @@
         <v>62</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="F6" s="66"/>
-    </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>56</v>
       </c>
@@ -1761,10 +1690,10 @@
         <v>64</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>57</v>
       </c>
@@ -1778,38 +1707,38 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="58"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="59"/>
-      <c r="D12" s="60"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="56"/>
+      <c r="D12" s="57"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="62"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="58"/>
+      <c r="D13" s="59"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>3</v>
       </c>
@@ -1823,7 +1752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>69</v>
       </c>
@@ -1842,31 +1771,31 @@
       <c r="A18" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="57"/>
-      <c r="D18" s="58"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="61"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="60"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="62"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="59"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
@@ -1982,31 +1911,31 @@
       <c r="A30" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="57" t="s">
+      <c r="B30" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="58"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="61"/>
     </row>
     <row r="31" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="59" t="s">
+      <c r="B31" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="C31" s="59"/>
-      <c r="D31" s="60"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="57"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="61" t="s">
+      <c r="B32" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="62"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="59"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
@@ -2083,31 +2012,31 @@
       <c r="A40" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="57" t="s">
+      <c r="B40" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="57"/>
-      <c r="D40" s="58"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="61"/>
     </row>
     <row r="41" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="59" t="s">
+      <c r="B41" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="59"/>
-      <c r="D41" s="60"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="57"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="61" t="s">
-        <v>218</v>
-      </c>
-      <c r="C42" s="61"/>
-      <c r="D42" s="62"/>
+      <c r="B42" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="C42" s="58"/>
+      <c r="D42" s="59"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
@@ -2145,7 +2074,7 @@
         <v>95</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>97</v>
@@ -2153,13 +2082,13 @@
     </row>
     <row r="46" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="21" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B46" s="13" t="s">
         <v>153</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>83</v>
@@ -2170,31 +2099,31 @@
       <c r="A49" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="57" t="s">
+      <c r="B49" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="C49" s="57"/>
-      <c r="D49" s="58"/>
+      <c r="C49" s="60"/>
+      <c r="D49" s="61"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B50" s="59" t="s">
+      <c r="B50" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="59"/>
-      <c r="D50" s="60"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="57"/>
     </row>
     <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="61" t="s">
+      <c r="B51" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C51" s="61"/>
-      <c r="D51" s="62"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="59"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
@@ -2271,31 +2200,31 @@
       <c r="A59" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B59" s="57" t="s">
+      <c r="B59" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="C59" s="57"/>
-      <c r="D59" s="58"/>
+      <c r="C59" s="60"/>
+      <c r="D59" s="61"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="59" t="s">
+      <c r="B60" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="59"/>
-      <c r="D60" s="60"/>
+      <c r="C60" s="56"/>
+      <c r="D60" s="57"/>
     </row>
     <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="61" t="s">
+      <c r="B61" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="C61" s="61"/>
-      <c r="D61" s="62"/>
+      <c r="C61" s="58"/>
+      <c r="D61" s="59"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
@@ -2344,31 +2273,31 @@
       <c r="A67" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B67" s="57" t="s">
+      <c r="B67" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="C67" s="57"/>
-      <c r="D67" s="58"/>
+      <c r="C67" s="60"/>
+      <c r="D67" s="61"/>
     </row>
     <row r="68" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B68" s="59" t="s">
+      <c r="B68" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="C68" s="59"/>
-      <c r="D68" s="60"/>
+      <c r="C68" s="56"/>
+      <c r="D68" s="57"/>
     </row>
     <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B69" s="61" t="s">
+      <c r="B69" s="58" t="s">
         <v>175</v>
       </c>
-      <c r="C69" s="61"/>
-      <c r="D69" s="62"/>
+      <c r="C69" s="58"/>
+      <c r="D69" s="59"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
@@ -2406,7 +2335,7 @@
         <v>107</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D72" s="12" t="s">
         <v>97</v>
@@ -2414,13 +2343,13 @@
     </row>
     <row r="73" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="21" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>153</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D73" s="14" t="s">
         <v>83</v>
@@ -2431,31 +2360,31 @@
       <c r="A76" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B76" s="57" t="s">
+      <c r="B76" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="C76" s="57"/>
-      <c r="D76" s="58"/>
+      <c r="C76" s="60"/>
+      <c r="D76" s="61"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B77" s="59" t="s">
+      <c r="B77" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="C77" s="59"/>
-      <c r="D77" s="60"/>
+      <c r="C77" s="56"/>
+      <c r="D77" s="57"/>
     </row>
     <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B78" s="61" t="s">
+      <c r="B78" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C78" s="61"/>
-      <c r="D78" s="62"/>
+      <c r="C78" s="58"/>
+      <c r="D78" s="59"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
@@ -2574,31 +2503,31 @@
       <c r="A89" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B89" s="57" t="s">
+      <c r="B89" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="C89" s="57"/>
-      <c r="D89" s="58"/>
+      <c r="C89" s="60"/>
+      <c r="D89" s="61"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B90" s="59" t="s">
+      <c r="B90" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="C90" s="59"/>
-      <c r="D90" s="60"/>
+      <c r="C90" s="56"/>
+      <c r="D90" s="57"/>
     </row>
     <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B91" s="61" t="s">
+      <c r="B91" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C91" s="61"/>
-      <c r="D91" s="62"/>
+      <c r="C91" s="58"/>
+      <c r="D91" s="59"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
@@ -2675,31 +2604,31 @@
       <c r="A99" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B99" s="57" t="s">
+      <c r="B99" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="C99" s="57"/>
-      <c r="D99" s="58"/>
+      <c r="C99" s="60"/>
+      <c r="D99" s="61"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B100" s="59" t="s">
+      <c r="B100" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="C100" s="59"/>
-      <c r="D100" s="60"/>
+      <c r="C100" s="56"/>
+      <c r="D100" s="57"/>
     </row>
     <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B101" s="61" t="s">
+      <c r="B101" s="58" t="s">
         <v>146</v>
       </c>
-      <c r="C101" s="61"/>
-      <c r="D101" s="62"/>
+      <c r="C101" s="58"/>
+      <c r="D101" s="59"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
@@ -2734,31 +2663,31 @@
       <c r="A106" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B106" s="57" t="s">
+      <c r="B106" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="C106" s="57"/>
-      <c r="D106" s="58"/>
+      <c r="C106" s="60"/>
+      <c r="D106" s="61"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B107" s="59" t="s">
+      <c r="B107" s="56" t="s">
         <v>150</v>
       </c>
-      <c r="C107" s="59"/>
-      <c r="D107" s="60"/>
+      <c r="C107" s="56"/>
+      <c r="D107" s="57"/>
     </row>
     <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B108" s="61" t="s">
+      <c r="B108" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C108" s="61"/>
-      <c r="D108" s="62"/>
+      <c r="C108" s="58"/>
+      <c r="D108" s="59"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
@@ -2821,31 +2750,31 @@
       <c r="A115" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B115" s="57" t="s">
+      <c r="B115" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="C115" s="57"/>
-      <c r="D115" s="58"/>
+      <c r="C115" s="60"/>
+      <c r="D115" s="61"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B116" s="59" t="s">
+      <c r="B116" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="C116" s="59"/>
-      <c r="D116" s="60"/>
+      <c r="C116" s="56"/>
+      <c r="D116" s="57"/>
     </row>
     <row r="117" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B117" s="61" t="s">
+      <c r="B117" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="C117" s="61"/>
-      <c r="D117" s="62"/>
+      <c r="C117" s="58"/>
+      <c r="D117" s="59"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
@@ -2922,31 +2851,31 @@
       <c r="A125" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B125" s="57" t="s">
+      <c r="B125" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="C125" s="57"/>
-      <c r="D125" s="58"/>
+      <c r="C125" s="60"/>
+      <c r="D125" s="61"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B126" s="59" t="s">
+      <c r="B126" s="56" t="s">
         <v>170</v>
       </c>
-      <c r="C126" s="59"/>
-      <c r="D126" s="60"/>
+      <c r="C126" s="56"/>
+      <c r="D126" s="57"/>
     </row>
     <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B127" s="61" t="s">
+      <c r="B127" s="58" t="s">
         <v>172</v>
       </c>
-      <c r="C127" s="61"/>
-      <c r="D127" s="62"/>
+      <c r="C127" s="58"/>
+      <c r="D127" s="59"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
@@ -2995,31 +2924,31 @@
       <c r="A133" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B133" s="57" t="s">
+      <c r="B133" s="60" t="s">
         <v>173</v>
       </c>
-      <c r="C133" s="57"/>
-      <c r="D133" s="58"/>
+      <c r="C133" s="60"/>
+      <c r="D133" s="61"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B134" s="59" t="s">
+      <c r="B134" s="56" t="s">
         <v>174</v>
       </c>
-      <c r="C134" s="59"/>
-      <c r="D134" s="60"/>
+      <c r="C134" s="56"/>
+      <c r="D134" s="57"/>
     </row>
     <row r="135" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B135" s="61" t="s">
+      <c r="B135" s="58" t="s">
         <v>175</v>
       </c>
-      <c r="C135" s="61"/>
-      <c r="D135" s="62"/>
+      <c r="C135" s="58"/>
+      <c r="D135" s="59"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
@@ -3068,31 +2997,31 @@
       <c r="A141" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B141" s="57" t="s">
+      <c r="B141" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="C141" s="57"/>
-      <c r="D141" s="58"/>
+      <c r="C141" s="60"/>
+      <c r="D141" s="61"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B142" s="59" t="s">
+      <c r="B142" s="56" t="s">
         <v>178</v>
       </c>
-      <c r="C142" s="59"/>
-      <c r="D142" s="60"/>
+      <c r="C142" s="56"/>
+      <c r="D142" s="57"/>
     </row>
     <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B143" s="61" t="s">
+      <c r="B143" s="58" t="s">
         <v>179</v>
       </c>
-      <c r="C143" s="61"/>
-      <c r="D143" s="62"/>
+      <c r="C143" s="58"/>
+      <c r="D143" s="59"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="8" t="s">
@@ -3141,31 +3070,31 @@
       <c r="A149" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B149" s="57" t="s">
+      <c r="B149" s="60" t="s">
         <v>181</v>
       </c>
-      <c r="C149" s="57"/>
-      <c r="D149" s="58"/>
+      <c r="C149" s="60"/>
+      <c r="D149" s="61"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B150" s="59" t="s">
+      <c r="B150" s="56" t="s">
         <v>182</v>
       </c>
-      <c r="C150" s="59"/>
-      <c r="D150" s="60"/>
+      <c r="C150" s="56"/>
+      <c r="D150" s="57"/>
     </row>
     <row r="151" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B151" s="61" t="s">
+      <c r="B151" s="58" t="s">
         <v>183</v>
       </c>
-      <c r="C151" s="61"/>
-      <c r="D151" s="62"/>
+      <c r="C151" s="58"/>
+      <c r="D151" s="59"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
@@ -3214,31 +3143,31 @@
       <c r="A157" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B157" s="57" t="s">
+      <c r="B157" s="60" t="s">
         <v>185</v>
       </c>
-      <c r="C157" s="57"/>
-      <c r="D157" s="58"/>
+      <c r="C157" s="60"/>
+      <c r="D157" s="61"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B158" s="59" t="s">
+      <c r="B158" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="C158" s="59"/>
-      <c r="D158" s="60"/>
+      <c r="C158" s="56"/>
+      <c r="D158" s="57"/>
     </row>
     <row r="159" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B159" s="61" t="s">
+      <c r="B159" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C159" s="61"/>
-      <c r="D159" s="62"/>
+      <c r="C159" s="58"/>
+      <c r="D159" s="59"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="8" t="s">
@@ -3301,31 +3230,31 @@
       <c r="A166" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B166" s="57" t="s">
+      <c r="B166" s="60" t="s">
         <v>193</v>
       </c>
-      <c r="C166" s="57"/>
-      <c r="D166" s="58"/>
+      <c r="C166" s="60"/>
+      <c r="D166" s="61"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B167" s="59" t="s">
+      <c r="B167" s="56" t="s">
         <v>194</v>
       </c>
-      <c r="C167" s="59"/>
-      <c r="D167" s="60"/>
+      <c r="C167" s="56"/>
+      <c r="D167" s="57"/>
     </row>
     <row r="168" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B168" s="61" t="s">
+      <c r="B168" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="C168" s="61"/>
-      <c r="D168" s="62"/>
+      <c r="C168" s="58"/>
+      <c r="D168" s="59"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="8" t="s">
@@ -3366,18 +3295,18 @@
         <v>199</v>
       </c>
       <c r="D171" s="12" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="41" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B172" s="11" t="s">
         <v>63</v>
       </c>
       <c r="C172" s="11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D172" s="12"/>
     </row>
@@ -3389,7 +3318,7 @@
         <v>107</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D173" s="14" t="s">
         <v>168</v>
@@ -3400,31 +3329,31 @@
       <c r="A176" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B176" s="57" t="s">
-        <v>203</v>
-      </c>
-      <c r="C176" s="57"/>
-      <c r="D176" s="58"/>
-    </row>
-    <row r="177" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B176" s="60" t="s">
+        <v>204</v>
+      </c>
+      <c r="C176" s="60"/>
+      <c r="D176" s="61"/>
+    </row>
+    <row r="177" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B177" s="59" t="s">
-        <v>204</v>
-      </c>
-      <c r="C177" s="59"/>
-      <c r="D177" s="60"/>
+      <c r="B177" s="56" t="s">
+        <v>205</v>
+      </c>
+      <c r="C177" s="56"/>
+      <c r="D177" s="57"/>
     </row>
     <row r="178" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B178" s="61" t="s">
-        <v>206</v>
-      </c>
-      <c r="C178" s="61"/>
-      <c r="D178" s="62"/>
+      <c r="B178" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="C178" s="58"/>
+      <c r="D178" s="59"/>
     </row>
     <row r="179" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="50" t="s">
@@ -3442,7 +3371,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="53" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B180" s="54" t="s">
         <v>195</v>
@@ -3451,7 +3380,7 @@
         <v>196</v>
       </c>
       <c r="D180" s="55" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3459,195 +3388,91 @@
         <v>94</v>
       </c>
       <c r="B181" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C181" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="D181" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C181" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="D181" s="12" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A182" s="63" t="s">
-        <v>101</v>
-      </c>
-      <c r="B182" s="64" t="s">
-        <v>58</v>
-      </c>
-      <c r="C182" s="56" t="s">
-        <v>222</v>
-      </c>
-      <c r="D182" s="65" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="B183" s="13" t="s">
+    </row>
+    <row r="182" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="C183" s="13" t="s">
+      <c r="B182" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="D183" s="14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B186" s="57" t="s">
-        <v>219</v>
-      </c>
-      <c r="C186" s="57"/>
-      <c r="D186" s="58"/>
-    </row>
-    <row r="187" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B187" s="59" t="s">
-        <v>220</v>
-      </c>
-      <c r="C187" s="59"/>
-      <c r="D187" s="60"/>
-    </row>
-    <row r="188" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B188" s="61" t="s">
-        <v>206</v>
-      </c>
-      <c r="C188" s="61"/>
-      <c r="D188" s="62"/>
-    </row>
-    <row r="189" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="B189" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C189" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D189" s="52" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="53" t="s">
-        <v>205</v>
-      </c>
-      <c r="B190" s="54" t="s">
-        <v>195</v>
-      </c>
-      <c r="C190" s="54" t="s">
-        <v>196</v>
-      </c>
-      <c r="D190" s="55" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A191" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="B191" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C191" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="D191" s="12" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A192" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="B192" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="C192" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="D192" s="14" t="s">
-        <v>221</v>
+      <c r="C182" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="D182" s="14" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="63">
-    <mergeCell ref="B186:D186"/>
-    <mergeCell ref="B187:D187"/>
-    <mergeCell ref="B188:D188"/>
+  <mergeCells count="60">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="B100:D100"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B106:D106"/>
+    <mergeCell ref="B107:D107"/>
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="B115:D115"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="B125:D125"/>
+    <mergeCell ref="B126:D126"/>
+    <mergeCell ref="B127:D127"/>
+    <mergeCell ref="B133:D133"/>
+    <mergeCell ref="B134:D134"/>
+    <mergeCell ref="B135:D135"/>
+    <mergeCell ref="B141:D141"/>
+    <mergeCell ref="B142:D142"/>
+    <mergeCell ref="B143:D143"/>
+    <mergeCell ref="B149:D149"/>
+    <mergeCell ref="B150:D150"/>
+    <mergeCell ref="B151:D151"/>
+    <mergeCell ref="B157:D157"/>
+    <mergeCell ref="B158:D158"/>
+    <mergeCell ref="B159:D159"/>
+    <mergeCell ref="B166:D166"/>
     <mergeCell ref="B167:D167"/>
     <mergeCell ref="B168:D168"/>
     <mergeCell ref="B176:D176"/>
     <mergeCell ref="B177:D177"/>
     <mergeCell ref="B178:D178"/>
-    <mergeCell ref="B151:D151"/>
-    <mergeCell ref="B157:D157"/>
-    <mergeCell ref="B158:D158"/>
-    <mergeCell ref="B159:D159"/>
-    <mergeCell ref="B166:D166"/>
-    <mergeCell ref="B141:D141"/>
-    <mergeCell ref="B142:D142"/>
-    <mergeCell ref="B143:D143"/>
-    <mergeCell ref="B149:D149"/>
-    <mergeCell ref="B150:D150"/>
-    <mergeCell ref="B126:D126"/>
-    <mergeCell ref="B127:D127"/>
-    <mergeCell ref="B133:D133"/>
-    <mergeCell ref="B134:D134"/>
-    <mergeCell ref="B135:D135"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="B115:D115"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="B125:D125"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="B100:D100"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B106:D106"/>
-    <mergeCell ref="B107:D107"/>
-    <mergeCell ref="B77:D77"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="B91:D91"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>